<commit_message>
GA_Only and PSO_Only folders
</commit_message>
<xml_diff>
--- a/code/BestCost.xlsx
+++ b/code/BestCost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OneDrive - SOCIEDADE DE ENSINO SUPERIOR ESTACIO DE SA\GitHub Desktop\14Bus-Parallel-Optimization\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04E8445-6B61-408A-BF4A-732F40A79EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6AE9E0-470E-4D11-88CE-4385D821DB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19080" yWindow="2655" windowWidth="12930" windowHeight="11385" xr2:uid="{D0A93FD4-D13B-42E5-9269-115999F2EC85}"/>
+    <workbookView xWindow="19080" yWindow="2655" windowWidth="12930" windowHeight="11385" xr2:uid="{A44FC4E6-98EB-49A4-9557-162D7931F20A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -379,7 +379,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{479BC6A8-FAB3-4A71-96C5-0D82A3790D91}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E2B2EC-CC29-4F31-87A5-7D889B129188}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -388,7 +388,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>34194.096458353641</v>
+        <v>33915.575708084776</v>
       </c>
     </row>
   </sheetData>

</xml_diff>